<commit_message>
analyze arup quant dist with IC grouping
</commit_message>
<xml_diff>
--- a/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
+++ b/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonischwarz/Box/Synergy Laboratories Co-Development Projects/UTI Test/Collaboration Experiments/R&amp;D Lab Exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmontgomery/OneDrive/Documents/IDbyDNA/Code/AbsoluteQuantification/arup_urine_samples_ge_study/ge_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407ACF71-06C3-334E-9911-AB4E38B4BB87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E556E4AD-343B-1544-8E24-ADCC0AA7034D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36700" yWindow="460" windowWidth="32920" windowHeight="18780" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Log" sheetId="1" r:id="rId1"/>
@@ -548,9 +548,6 @@
     <t>63.92</t>
   </si>
   <si>
-    <t>IDBD-D100385</t>
-  </si>
-  <si>
     <t>IDbyDNA-5400</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>IDBD-D100386</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38306794-63FA-0746-9C8B-867300C82BA0}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3940,13 +3940,13 @@
         <v>117</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>26</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="52" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D52" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>88</v>
@@ -4034,7 +4034,7 @@
       <c r="P52" s="11"/>
       <c r="Q52" s="11"/>
       <c r="R52" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S52" s="11" t="s">
         <v>34</v>
@@ -4045,10 +4045,10 @@
     </row>
     <row r="53" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D53" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>26</v>
@@ -4083,7 +4083,7 @@
       <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
       <c r="R53" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S53" s="11" t="s">
         <v>34</v>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="54" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D54" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>154</v>
@@ -4132,7 +4132,7 @@
       <c r="P54" s="11"/>
       <c r="Q54" s="11"/>
       <c r="R54" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S54" s="11" t="s">
         <v>34</v>
@@ -4143,7 +4143,7 @@
     </row>
     <row r="55" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D55" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>96</v>
@@ -4181,7 +4181,7 @@
       <c r="P55" s="11"/>
       <c r="Q55" s="11"/>
       <c r="R55" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S55" s="11" t="s">
         <v>34</v>
@@ -4192,10 +4192,10 @@
     </row>
     <row r="56" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D56" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>26</v>
@@ -4213,7 +4213,7 @@
         <v>107.95</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L56" s="11"/>
       <c r="M56" s="11" t="s">
@@ -4228,7 +4228,7 @@
       <c r="P56" s="11"/>
       <c r="Q56" s="11"/>
       <c r="R56" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S56" s="11" t="s">
         <v>34</v>
@@ -4239,10 +4239,10 @@
     </row>
     <row r="57" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D57" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>26</v>
@@ -4277,7 +4277,7 @@
       <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
       <c r="R57" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S57" s="11" t="s">
         <v>34</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="58" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D58" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>26</v>
@@ -4326,7 +4326,7 @@
       <c r="P58" s="11"/>
       <c r="Q58" s="11"/>
       <c r="R58" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S58" s="11" t="s">
         <v>34</v>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="59" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D59" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>98</v>
@@ -4375,10 +4375,10 @@
       <c r="P59" s="11"/>
       <c r="Q59" s="11"/>
       <c r="R59" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="S59" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="S59" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="T59" s="11" t="s">
         <v>35</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="60" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D60" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E60" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>102</v>
@@ -4424,7 +4424,7 @@
       <c r="P60" s="11"/>
       <c r="Q60" s="11"/>
       <c r="R60" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S60" s="11" t="s">
         <v>112</v>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="61" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D61" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E61" s="11">
         <v>75</v>
@@ -4456,7 +4456,7 @@
         <v>51.6</v>
       </c>
       <c r="K61" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>40</v>
@@ -4473,10 +4473,10 @@
       <c r="P61" s="11"/>
       <c r="Q61" s="11"/>
       <c r="R61" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="S61" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="S61" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="T61" s="11" t="s">
         <v>35</v>
@@ -4484,10 +4484,10 @@
     </row>
     <row r="62" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D62" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E62" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>102</v>
@@ -4522,10 +4522,10 @@
       <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
       <c r="R62" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="S62" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="S62" s="11" t="s">
-        <v>200</v>
       </c>
       <c r="T62" s="11" t="s">
         <v>35</v>
@@ -4533,10 +4533,10 @@
     </row>
     <row r="63" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D63" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>102</v>
@@ -4554,7 +4554,7 @@
         <v>35.630000000000003</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L63" s="11"/>
       <c r="M63" s="11" t="s">
@@ -4569,10 +4569,10 @@
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
       <c r="R63" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="S63" s="11" t="s">
         <v>202</v>
-      </c>
-      <c r="S63" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="T63" s="11" t="s">
         <v>35</v>
@@ -4580,7 +4580,7 @@
     </row>
     <row r="64" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D64" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>104</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="65" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D65" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>60</v>
@@ -4667,10 +4667,10 @@
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
       <c r="R65" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="S65" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="S65" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="T65" s="11" t="s">
         <v>35</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="66" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D66" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>56</v>
@@ -4716,10 +4716,10 @@
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
       <c r="R66" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="S66" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="S66" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="T66" s="11" t="s">
         <v>35</v>
@@ -4727,10 +4727,10 @@
     </row>
     <row r="67" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="D67" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>26</v>
@@ -4765,10 +4765,10 @@
       <c r="P67" s="11"/>
       <c r="Q67" s="11"/>
       <c r="R67" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="S67" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="S67" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="T67" s="11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
updated arup sample processing log
</commit_message>
<xml_diff>
--- a/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
+++ b/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmontgomery/OneDrive/Documents/IDbyDNA/Code/AbsoluteQuantification/arup_urine_samples_ge_study/ge_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E556E4AD-343B-1544-8E24-ADCC0AA7034D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBC8BF23-3D1E-F34E-9C35-E3BE99BB96DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="253">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -698,6 +698,126 @@
     <t>22</t>
   </si>
   <si>
+    <t>190903B01</t>
+  </si>
+  <si>
+    <t>IDBD-D100397</t>
+  </si>
+  <si>
+    <t>IDBD-D100398</t>
+  </si>
+  <si>
+    <t>IDBD-D100399</t>
+  </si>
+  <si>
+    <t>IDBD-D100400</t>
+  </si>
+  <si>
+    <t>IDBD-D100401</t>
+  </si>
+  <si>
+    <t>IDBD-D100402</t>
+  </si>
+  <si>
+    <t>IDBD-D100403</t>
+  </si>
+  <si>
+    <t>IDBD-D100404</t>
+  </si>
+  <si>
+    <t>IDBD-D100405</t>
+  </si>
+  <si>
+    <t>IDBD-D100406</t>
+  </si>
+  <si>
+    <t>IDBD-D100407</t>
+  </si>
+  <si>
+    <t>IDBD-D100408</t>
+  </si>
+  <si>
+    <t>IDBD-D100409</t>
+  </si>
+  <si>
+    <t>IDBD-D100410</t>
+  </si>
+  <si>
+    <t>IDBD-D100444</t>
+  </si>
+  <si>
+    <t>IDBD-D100445</t>
+  </si>
+  <si>
+    <t>IDBD-D100450</t>
+  </si>
+  <si>
+    <t>IDBD-D100451</t>
+  </si>
+  <si>
+    <t>IDBD-D100452</t>
+  </si>
+  <si>
+    <t>IDBD-D100453</t>
+  </si>
+  <si>
+    <t>190904-2-1</t>
+  </si>
+  <si>
+    <t>190904-1-1</t>
+  </si>
+  <si>
+    <t>190903B02</t>
+  </si>
+  <si>
+    <t>IDBD-D100455</t>
+  </si>
+  <si>
+    <t>IDBD-D100456</t>
+  </si>
+  <si>
+    <t>IDBD-D100457</t>
+  </si>
+  <si>
+    <t>IDBD-D100460</t>
+  </si>
+  <si>
+    <t>IDBD-D100458</t>
+  </si>
+  <si>
+    <t>IDBD-D100459</t>
+  </si>
+  <si>
+    <t>IDBD-D100446</t>
+  </si>
+  <si>
+    <t>IDBD-D100440</t>
+  </si>
+  <si>
+    <t>IDBD-D100441</t>
+  </si>
+  <si>
+    <t>IDBD-D100454</t>
+  </si>
+  <si>
+    <t>IDBD-D100442</t>
+  </si>
+  <si>
+    <t>IDBD-D100447</t>
+  </si>
+  <si>
+    <t>IDBD-D100443</t>
+  </si>
+  <si>
+    <t>IDBD-D100448</t>
+  </si>
+  <si>
+    <t>IDBD-D100438</t>
+  </si>
+  <si>
+    <t>IDBD-D100439</t>
+  </si>
+  <si>
     <t>IDBD-D100386</t>
   </si>
 </sst>
@@ -705,7 +825,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -744,8 +864,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -778,12 +921,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -834,11 +982,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD5D3D1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD5D3D1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD5D3D1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD5D3D1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -858,16 +1021,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
@@ -877,6 +1030,24 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1194,87 +1365,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38306794-63FA-0746-9C8B-867300C82BA0}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="11.5" style="13"/>
-    <col min="4" max="4" width="16" style="13" customWidth="1"/>
-    <col min="5" max="10" width="11.5" style="13"/>
-    <col min="11" max="11" width="32.6640625" style="13" customWidth="1"/>
-    <col min="12" max="17" width="11.5" style="13"/>
-    <col min="18" max="18" width="73.1640625" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="11.5" style="13"/>
+    <col min="1" max="2" width="11.5" style="9"/>
+    <col min="3" max="3" width="18.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16" style="9" customWidth="1"/>
+    <col min="5" max="10" width="11.5" style="9"/>
+    <col min="11" max="11" width="32.6640625" style="9" customWidth="1"/>
+    <col min="12" max="17" width="11.5" style="9"/>
+    <col min="18" max="18" width="73.1640625" style="9" customWidth="1"/>
+    <col min="19" max="16384" width="11.5" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="44" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1287,52 +1459,52 @@
       <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="14">
-        <v>2019</v>
-      </c>
-      <c r="I2" s="14">
+      <c r="G2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="10">
+        <v>2019</v>
+      </c>
+      <c r="I2" s="10">
         <v>4.12</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="10">
         <v>68.900000000000006</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14" t="s">
+      <c r="O2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="S2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1620,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1506,7 +1678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1564,7 +1736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1622,7 +1794,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1680,7 +1852,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1738,7 +1910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="5" customFormat="1" ht="16">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1852,7 +2024,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="5" customFormat="1" ht="16">
+      <c r="A12" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>213</v>
+      </c>
       <c r="D12" s="6" t="s">
         <v>73</v>
       </c>
@@ -1901,7 +2082,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="5" customFormat="1" ht="16">
+      <c r="A13" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>214</v>
+      </c>
       <c r="D13" s="6" t="s">
         <v>76</v>
       </c>
@@ -1950,7 +2140,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="5" customFormat="1" ht="16">
+      <c r="A14" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>215</v>
+      </c>
       <c r="D14" s="6" t="s">
         <v>78</v>
       </c>
@@ -1999,7 +2198,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="5" customFormat="1" ht="16">
+      <c r="A15" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>216</v>
+      </c>
       <c r="D15" s="6" t="s">
         <v>80</v>
       </c>
@@ -2048,7 +2256,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="5" customFormat="1" ht="16">
+      <c r="A16" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>217</v>
+      </c>
       <c r="D16" s="6" t="s">
         <v>82</v>
       </c>
@@ -2097,7 +2314,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A17" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>218</v>
+      </c>
       <c r="D17" s="6" t="s">
         <v>84</v>
       </c>
@@ -2146,7 +2372,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A18" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>219</v>
+      </c>
       <c r="D18" s="6" t="s">
         <v>85</v>
       </c>
@@ -2195,7 +2430,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A19" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>220</v>
+      </c>
       <c r="D19" s="6" t="s">
         <v>87</v>
       </c>
@@ -2244,7 +2488,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A20" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>221</v>
+      </c>
       <c r="D20" s="6" t="s">
         <v>90</v>
       </c>
@@ -2293,7 +2546,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A21" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>222</v>
+      </c>
       <c r="D21" s="6" t="s">
         <v>93</v>
       </c>
@@ -2342,7 +2604,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A22" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>223</v>
+      </c>
       <c r="D22" s="6" t="s">
         <v>95</v>
       </c>
@@ -2391,7 +2662,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A23" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>224</v>
+      </c>
       <c r="D23" s="6" t="s">
         <v>97</v>
       </c>
@@ -2438,7 +2718,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A24" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>225</v>
+      </c>
       <c r="D24" s="6" t="s">
         <v>99</v>
       </c>
@@ -2487,7 +2776,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A25" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>226</v>
+      </c>
       <c r="D25" s="6" t="s">
         <v>101</v>
       </c>
@@ -2536,7 +2834,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A26" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>229</v>
+      </c>
       <c r="D26" s="6" t="s">
         <v>103</v>
       </c>
@@ -2585,7 +2892,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A27" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>230</v>
+      </c>
       <c r="D27" s="6" t="s">
         <v>106</v>
       </c>
@@ -2634,7 +2950,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A28" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>231</v>
+      </c>
       <c r="D28" s="6" t="s">
         <v>108</v>
       </c>
@@ -2683,7 +3008,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A29" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>227</v>
+      </c>
       <c r="D29" s="6" t="s">
         <v>110</v>
       </c>
@@ -2732,7 +3066,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A30" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>228</v>
+      </c>
       <c r="D30" s="6" t="s">
         <v>113</v>
       </c>
@@ -2781,7 +3124,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" s="5" customFormat="1" ht="16">
+      <c r="A31" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>232</v>
+      </c>
       <c r="D31" s="6" t="s">
         <v>114</v>
       </c>
@@ -2830,7 +3182,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
         <v>116</v>
       </c>
@@ -2888,7 +3240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
         <v>116</v>
       </c>
@@ -2946,7 +3298,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A34" s="5" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
         <v>116</v>
       </c>
@@ -3062,7 +3414,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
         <v>116</v>
       </c>
@@ -3120,7 +3472,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A37" s="5" t="s">
         <v>116</v>
       </c>
@@ -3178,7 +3530,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3236,7 +3588,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
         <v>116</v>
       </c>
@@ -3294,7 +3646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
         <v>116</v>
       </c>
@@ -3352,7 +3704,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A41" s="5" t="s">
         <v>116</v>
       </c>
@@ -3410,7 +3762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A42" s="5" t="s">
         <v>116</v>
       </c>
@@ -3468,7 +3820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A43" s="5" t="s">
         <v>116</v>
       </c>
@@ -3524,7 +3876,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
         <v>116</v>
       </c>
@@ -3582,7 +3934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A45" s="5" t="s">
         <v>116</v>
       </c>
@@ -3640,7 +3992,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A46" s="5" t="s">
         <v>116</v>
       </c>
@@ -3696,7 +4048,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A47" s="5" t="s">
         <v>116</v>
       </c>
@@ -3754,7 +4106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" s="5" customFormat="1" ht="16">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -3812,7 +4164,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:24" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
         <v>116</v>
       </c>
@@ -3870,7 +4222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" s="8" customFormat="1" ht="16">
       <c r="A50" s="5" t="s">
         <v>116</v>
       </c>
@@ -3932,7 +4284,7 @@
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
     </row>
-    <row r="51" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:24" s="8" customFormat="1" ht="16">
       <c r="A51" s="5" t="s">
         <v>116</v>
       </c>
@@ -3940,7 +4292,7 @@
         <v>117</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>169</v>
@@ -3994,783 +4346,927 @@
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
     </row>
-    <row r="52" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D52" s="10" t="s">
+    <row r="52" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A52" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D52" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I52" s="11">
+      <c r="G52" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I52" s="17">
         <v>24.8</v>
       </c>
-      <c r="J52" s="11">
+      <c r="J52" s="17">
         <v>71.2</v>
       </c>
-      <c r="K52" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L52" s="11" t="s">
+      <c r="K52" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L52" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M52" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N52" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O52" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11" t="s">
+      <c r="M52" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O52" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="S52" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T52" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D53" s="10" t="s">
+      <c r="S52" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T52" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A53" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I53" s="11">
+      <c r="G53" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I53" s="17">
         <v>6.78</v>
       </c>
-      <c r="J53" s="11">
+      <c r="J53" s="17">
         <v>69.55</v>
       </c>
-      <c r="K53" s="11" t="s">
+      <c r="K53" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L53" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M53" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N53" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O53" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11" t="s">
+      <c r="L53" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O53" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="S53" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T53" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D54" s="10" t="s">
+      <c r="S53" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A54" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G54" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H54" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I54" s="11">
+      <c r="G54" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I54" s="17">
         <v>5.4</v>
       </c>
-      <c r="J54" s="11">
+      <c r="J54" s="17">
         <v>106.2</v>
       </c>
-      <c r="K54" s="11" t="s">
+      <c r="K54" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L54" s="11" t="s">
+      <c r="L54" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M54" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N54" s="11" t="s">
+      <c r="M54" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N54" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O54" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11" t="s">
+      <c r="O54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="S54" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T54" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D55" s="10" t="s">
+      <c r="S54" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T54" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A55" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G55" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H55" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I55" s="11">
+      <c r="G55" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I55" s="17">
         <v>1.83</v>
       </c>
-      <c r="J55" s="11">
+      <c r="J55" s="17">
         <v>73.98</v>
       </c>
-      <c r="K55" s="11" t="s">
+      <c r="K55" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L55" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M55" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N55" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O55" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11" t="s">
+      <c r="L55" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M55" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O55" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="S55" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T55" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D56" s="10" t="s">
+      <c r="S55" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T55" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A56" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="D56" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="E56" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G56" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H56" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I56" s="11">
+      <c r="G56" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I56" s="17">
         <v>16.32</v>
       </c>
-      <c r="J56" s="11">
+      <c r="J56" s="17">
         <v>107.95</v>
       </c>
-      <c r="K56" s="11" t="s">
+      <c r="K56" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N56" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O56" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11" t="s">
+      <c r="L56" s="17"/>
+      <c r="M56" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O56" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="S56" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T56" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D57" s="10" t="s">
+      <c r="S56" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T56" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A57" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H57" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I57" s="11">
+      <c r="H57" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I57" s="17">
         <v>22.47</v>
       </c>
-      <c r="J57" s="11">
+      <c r="J57" s="17">
         <v>119.07</v>
       </c>
-      <c r="K57" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L57" s="11" t="s">
+      <c r="K57" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L57" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M57" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N57" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O57" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11" t="s">
+      <c r="M57" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N57" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="S57" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T57" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D58" s="10" t="s">
+      <c r="S57" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T57" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A58" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G58" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H58" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I58" s="11">
+      <c r="G58" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I58" s="17">
         <v>5.2</v>
       </c>
-      <c r="J58" s="11">
+      <c r="J58" s="17">
         <v>84.07</v>
       </c>
-      <c r="K58" s="11" t="s">
+      <c r="K58" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L58" s="11" t="s">
+      <c r="L58" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M58" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N58" s="11" t="s">
+      <c r="M58" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N58" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O58" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11" t="s">
+      <c r="O58" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="S58" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T58" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D59" s="10" t="s">
+      <c r="S58" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T58" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A59" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E59" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G59" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H59" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I59" s="11">
+      <c r="G59" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I59" s="17">
         <v>1.78</v>
       </c>
-      <c r="J59" s="11">
+      <c r="J59" s="17">
         <v>29.68</v>
       </c>
-      <c r="K59" s="11" t="s">
+      <c r="K59" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L59" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M59" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N59" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O59" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11" t="s">
+      <c r="L59" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N59" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O59" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="S59" s="11" t="s">
+      <c r="S59" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="T59" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D60" s="10" t="s">
+      <c r="T59" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A60" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D60" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H60" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I60" s="11">
+      <c r="G60" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I60" s="17">
         <v>2.65</v>
       </c>
-      <c r="J60" s="11">
+      <c r="J60" s="17">
         <v>34.520000000000003</v>
       </c>
-      <c r="K60" s="11" t="s">
+      <c r="K60" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L60" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M60" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N60" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O60" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="11" t="s">
+      <c r="L60" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N60" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O60" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="S60" s="11" t="s">
+      <c r="S60" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="T60" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D61" s="10" t="s">
+      <c r="T60" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A61" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="D61" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="E61" s="11">
+      <c r="E61" s="17">
         <v>75</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G61" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H61" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I61" s="11">
+      <c r="G61" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I61" s="17">
         <v>17.399999999999999</v>
       </c>
-      <c r="J61" s="11">
+      <c r="J61" s="17">
         <v>51.6</v>
       </c>
-      <c r="K61" s="11" t="s">
+      <c r="K61" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="L61" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M61" s="11" t="s">
+      <c r="L61" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M61" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N61" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O61" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11" t="s">
+      <c r="N61" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O61" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S61" s="11" t="s">
+      <c r="S61" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="T61" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D62" s="10" t="s">
+      <c r="T61" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A62" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D62" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E62" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="F62" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G62" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H62" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I62" s="11">
+      <c r="G62" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I62" s="17">
         <v>6.58</v>
       </c>
-      <c r="J62" s="11">
+      <c r="J62" s="17">
         <v>45.2</v>
       </c>
-      <c r="K62" s="11" t="s">
+      <c r="K62" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="11" t="s">
+      <c r="L62" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M62" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N62" s="11" t="s">
+      <c r="M62" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N62" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O62" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P62" s="11"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11" t="s">
+      <c r="O62" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="S62" s="11" t="s">
+      <c r="S62" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="T62" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D63" s="12" t="s">
+      <c r="T62" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A63" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G63" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H63" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I63" s="11">
+      <c r="G63" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I63" s="17">
         <v>21.12</v>
       </c>
-      <c r="J63" s="11">
+      <c r="J63" s="17">
         <v>35.630000000000003</v>
       </c>
-      <c r="K63" s="11" t="s">
+      <c r="K63" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N63" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O63" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11" t="s">
+      <c r="L63" s="17"/>
+      <c r="M63" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N63" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O63" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="S63" s="11" t="s">
+      <c r="S63" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="T63" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D64" s="12" t="s">
+      <c r="T63" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" s="18" customFormat="1" ht="16">
+      <c r="A64" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D64" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G64" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H64" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I64" s="11">
+      <c r="G64" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I64" s="17">
         <v>6.47</v>
       </c>
-      <c r="J64" s="11">
+      <c r="J64" s="17">
         <v>24.33</v>
       </c>
-      <c r="K64" s="11" t="s">
+      <c r="K64" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L64" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M64" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N64" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O64" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11" t="s">
+      <c r="L64" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O64" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="S64" s="11" t="s">
+      <c r="S64" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="T64" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="65" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D65" s="10" t="s">
+      <c r="T64" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" s="18" customFormat="1" ht="16">
+      <c r="A65" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D65" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E65" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G65" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H65" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I65" s="11">
+      <c r="G65" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I65" s="17">
         <v>10.42</v>
       </c>
-      <c r="J65" s="11">
+      <c r="J65" s="17">
         <v>68.72</v>
       </c>
-      <c r="K65" s="11" t="s">
+      <c r="K65" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L65" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M65" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N65" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O65" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11" t="s">
+      <c r="L65" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O65" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="17"/>
+      <c r="R65" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="S65" s="11" t="s">
+      <c r="S65" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="T65" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="66" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D66" s="12" t="s">
+      <c r="T65" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" s="18" customFormat="1" ht="16">
+      <c r="A66" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D66" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G66" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H66" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I66" s="11">
+      <c r="G66" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I66" s="17">
         <v>6.33</v>
       </c>
-      <c r="J66" s="11">
+      <c r="J66" s="17">
         <v>62.32</v>
       </c>
-      <c r="K66" s="11" t="s">
+      <c r="K66" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L66" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M66" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N66" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O66" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11" t="s">
+      <c r="L66" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M66" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="S66" s="11" t="s">
+      <c r="S66" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="T66" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="4:20" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="D67" s="12" t="s">
+      <c r="T66" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" s="18" customFormat="1" ht="16">
+      <c r="A67" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D67" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E67" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G67" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H67" s="11">
-        <v>2019</v>
-      </c>
-      <c r="I67" s="11">
+      <c r="G67" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I67" s="17">
         <v>3.85</v>
       </c>
-      <c r="J67" s="11">
+      <c r="J67" s="17">
         <v>58.82</v>
       </c>
-      <c r="K67" s="11" t="s">
+      <c r="K67" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L67" s="11" t="s">
+      <c r="L67" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M67" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N67" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O67" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11" t="s">
+      <c r="M67" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N67" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O67" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="S67" s="11" t="s">
+      <c r="S67" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="T67" s="11" t="s">
+      <c r="T67" s="17" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setup for arup urine sample coverage analysis
</commit_message>
<xml_diff>
--- a/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
+++ b/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmontgomery/OneDrive/Documents/IDbyDNA/Code/AbsoluteQuantification/arup_urine_samples_ge_study/ge_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37C9639-7635-D642-88CE-A6D95DE8790B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAD534A-04AE-FA4C-BD9E-F0A9290B00D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sample Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample Log'!$A$1:$R$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample Log'!$A$1:$T$98</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="340">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -1301,7 +1301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1332,9 +1332,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,6 +1379,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38306794-63FA-0746-9C8B-867300C82BA0}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P53" workbookViewId="0">
-      <selection activeCell="V71" sqref="V71"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -1707,69 +1708,69 @@
     <col min="1" max="2" width="11.5" style="8"/>
     <col min="3" max="3" width="18.1640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="21" style="8" customWidth="1"/>
-    <col min="5" max="10" width="11.5" style="19"/>
-    <col min="11" max="11" width="32.6640625" style="19" customWidth="1"/>
-    <col min="12" max="15" width="11.5" style="19"/>
-    <col min="16" max="16" width="73.1640625" style="19" customWidth="1"/>
-    <col min="17" max="18" width="11.5" style="19"/>
+    <col min="5" max="10" width="11.5" style="18"/>
+    <col min="11" max="11" width="32.6640625" style="18" customWidth="1"/>
+    <col min="12" max="15" width="11.5" style="18"/>
+    <col min="16" max="16" width="73.1640625" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.5" style="18"/>
     <col min="19" max="19" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="11.5" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" ht="44" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="24" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -1783,73 +1784,79 @@
       <c r="A2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>138</v>
+      <c r="C2" s="33" t="s">
+        <v>140</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="23">
-        <v>2019</v>
-      </c>
-      <c r="I2" s="23">
-        <v>4.63</v>
-      </c>
-      <c r="J2" s="23">
-        <v>38.97</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="22">
+        <v>2019</v>
+      </c>
+      <c r="I2" s="22">
+        <v>7.18</v>
+      </c>
+      <c r="J2" s="22">
+        <v>38.9</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="23" t="s">
+      <c r="O2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>32</v>
+      <c r="Q2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2">
+        <v>325000</v>
+      </c>
+      <c r="T2">
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>135</v>
+      <c r="C3" s="33" t="s">
+        <v>143</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>23</v>
@@ -1861,22 +1868,20 @@
         <v>2019</v>
       </c>
       <c r="I3" s="13">
-        <v>3.7</v>
+        <v>5.13</v>
       </c>
       <c r="J3" s="13">
-        <v>62.38</v>
+        <v>38.770000000000003</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="L3" s="13"/>
       <c r="M3" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>29</v>
@@ -1890,24 +1895,28 @@
       <c r="R3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S3"/>
-      <c r="T3"/>
+      <c r="S3">
+        <v>900000</v>
+      </c>
+      <c r="T3" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="4" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>115</v>
+      <c r="C4" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>23</v>
@@ -1919,10 +1928,10 @@
         <v>2019</v>
       </c>
       <c r="I4" s="13">
-        <v>7.78</v>
+        <v>4.92</v>
       </c>
       <c r="J4" s="13">
-        <v>48.77</v>
+        <v>62.23</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>49</v>
@@ -1949,30 +1958,30 @@
         <v>32</v>
       </c>
       <c r="S4">
-        <v>1400000</v>
-      </c>
-      <c r="T4" t="s">
-        <v>328</v>
+        <v>425000</v>
+      </c>
+      <c r="T4">
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>118</v>
+      <c r="C5" s="33" t="s">
+        <v>149</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>24</v>
@@ -1981,16 +1990,16 @@
         <v>2019</v>
       </c>
       <c r="I5" s="13">
-        <v>22.02</v>
+        <v>6.97</v>
       </c>
       <c r="J5" s="13">
-        <v>47.95</v>
+        <v>55.65</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>37</v>
@@ -2011,27 +2020,27 @@
         <v>32</v>
       </c>
       <c r="S5">
-        <v>2200000</v>
+        <v>500000</v>
       </c>
       <c r="T5" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>120</v>
+      <c r="C6" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>23</v>
@@ -2043,17 +2052,15 @@
         <v>2019</v>
       </c>
       <c r="I6" s="13">
-        <v>2.58</v>
+        <v>6.93</v>
       </c>
       <c r="J6" s="13">
-        <v>50.47</v>
+        <v>38.07</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="L6" s="13"/>
       <c r="M6" s="13" t="s">
         <v>37</v>
       </c>
@@ -2073,30 +2080,30 @@
         <v>32</v>
       </c>
       <c r="S6">
-        <v>400000</v>
+        <v>900000</v>
       </c>
       <c r="T6" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>122</v>
+      <c r="C7" s="33" t="s">
+        <v>154</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>24</v>
@@ -2105,10 +2112,10 @@
         <v>2019</v>
       </c>
       <c r="I7" s="13">
-        <v>4.68</v>
+        <v>10.43</v>
       </c>
       <c r="J7" s="13">
-        <v>49.55</v>
+        <v>56.2</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>49</v>
@@ -2135,27 +2142,27 @@
         <v>32</v>
       </c>
       <c r="S7">
-        <v>1200000</v>
-      </c>
-      <c r="T7" t="s">
-        <v>331</v>
+        <v>105000</v>
+      </c>
+      <c r="T7">
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A8" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>125</v>
+      <c r="C8" s="33" t="s">
+        <v>156</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>23</v>
@@ -2167,22 +2174,22 @@
         <v>2019</v>
       </c>
       <c r="I8" s="13">
-        <v>7.05</v>
+        <v>7.13</v>
       </c>
       <c r="J8" s="13">
-        <v>42.43</v>
+        <v>55.65</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>29</v>
@@ -2197,27 +2204,27 @@
         <v>32</v>
       </c>
       <c r="S8">
-        <v>400000</v>
+        <v>1100000</v>
       </c>
       <c r="T8" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>128</v>
+      <c r="C9" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>23</v>
@@ -2229,10 +2236,10 @@
         <v>2019</v>
       </c>
       <c r="I9" s="13">
-        <v>3.12</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="J9" s="13">
-        <v>47.18</v>
+        <v>55.8</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>49</v>
@@ -2259,27 +2266,27 @@
         <v>32</v>
       </c>
       <c r="S9">
-        <v>1200000</v>
+        <v>700000</v>
       </c>
       <c r="T9" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>130</v>
+      <c r="C10" s="33" t="s">
+        <v>162</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>23</v>
@@ -2291,10 +2298,10 @@
         <v>2019</v>
       </c>
       <c r="I10" s="13">
-        <v>5.15</v>
-      </c>
-      <c r="J10" s="13">
-        <v>44.43</v>
+        <v>21.03</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>49</v>
@@ -2321,27 +2328,27 @@
         <v>32</v>
       </c>
       <c r="S10">
-        <v>1500000</v>
-      </c>
-      <c r="T10" t="s">
-        <v>332</v>
+        <v>100000</v>
+      </c>
+      <c r="T10">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>132</v>
+      <c r="C11" s="33" t="s">
+        <v>249</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>23</v>
@@ -2353,13 +2360,13 @@
         <v>2019</v>
       </c>
       <c r="I11" s="13">
-        <v>3.15</v>
+        <v>19.8</v>
       </c>
       <c r="J11" s="13">
-        <v>41.62</v>
+        <v>49.1</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>37</v>
@@ -2383,27 +2390,27 @@
         <v>32</v>
       </c>
       <c r="S11">
-        <v>1500000</v>
+        <v>1100000</v>
       </c>
       <c r="T11" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A12" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>140</v>
+      <c r="C12" s="26" t="s">
+        <v>138</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>23</v>
@@ -2415,16 +2422,16 @@
         <v>2019</v>
       </c>
       <c r="I12" s="13">
-        <v>7.18</v>
+        <v>4.63</v>
       </c>
       <c r="J12" s="13">
-        <v>38.9</v>
+        <v>38.97</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M12" s="13" t="s">
         <v>37</v>
@@ -2444,28 +2451,28 @@
       <c r="R12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S12">
-        <v>325000</v>
-      </c>
-      <c r="T12">
-        <v>325</v>
+      <c r="S12" s="8">
+        <v>1100000</v>
+      </c>
+      <c r="T12" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>143</v>
+      <c r="C13" s="26" t="s">
+        <v>135</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>23</v>
@@ -2477,20 +2484,22 @@
         <v>2019</v>
       </c>
       <c r="I13" s="13">
-        <v>5.13</v>
+        <v>3.7</v>
       </c>
       <c r="J13" s="13">
-        <v>38.770000000000003</v>
+        <v>62.38</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="M13" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O13" s="13" t="s">
         <v>29</v>
@@ -2505,27 +2514,27 @@
         <v>32</v>
       </c>
       <c r="S13">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="T13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>146</v>
+      <c r="C14" s="26" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>23</v>
@@ -2537,10 +2546,10 @@
         <v>2019</v>
       </c>
       <c r="I14" s="13">
-        <v>4.92</v>
+        <v>7.78</v>
       </c>
       <c r="J14" s="13">
-        <v>62.23</v>
+        <v>48.77</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>49</v>
@@ -2567,30 +2576,30 @@
         <v>32</v>
       </c>
       <c r="S14">
-        <v>425000</v>
-      </c>
-      <c r="T14">
-        <v>425</v>
+        <v>1400000</v>
+      </c>
+      <c r="T14" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A15" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>149</v>
+      <c r="C15" s="26" t="s">
+        <v>118</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>24</v>
@@ -2599,16 +2608,16 @@
         <v>2019</v>
       </c>
       <c r="I15" s="13">
-        <v>6.97</v>
+        <v>22.02</v>
       </c>
       <c r="J15" s="13">
-        <v>55.65</v>
+        <v>47.95</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>37</v>
@@ -2629,27 +2638,27 @@
         <v>32</v>
       </c>
       <c r="S15">
-        <v>500000</v>
+        <v>2200000</v>
       </c>
       <c r="T15" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>152</v>
+      <c r="C16" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>23</v>
@@ -2661,15 +2670,17 @@
         <v>2019</v>
       </c>
       <c r="I16" s="13">
-        <v>6.93</v>
+        <v>2.58</v>
       </c>
       <c r="J16" s="13">
-        <v>38.07</v>
+        <v>50.47</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="M16" s="13" t="s">
         <v>37</v>
       </c>
@@ -2689,30 +2700,30 @@
         <v>32</v>
       </c>
       <c r="S16">
-        <v>900000</v>
+        <v>400000</v>
       </c>
       <c r="T16" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>154</v>
+      <c r="C17" s="26" t="s">
+        <v>122</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>24</v>
@@ -2721,10 +2732,10 @@
         <v>2019</v>
       </c>
       <c r="I17" s="13">
-        <v>10.43</v>
+        <v>4.68</v>
       </c>
       <c r="J17" s="13">
-        <v>56.2</v>
+        <v>49.55</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>49</v>
@@ -2751,27 +2762,27 @@
         <v>32</v>
       </c>
       <c r="S17">
-        <v>105000</v>
-      </c>
-      <c r="T17">
-        <v>105</v>
+        <v>1200000</v>
+      </c>
+      <c r="T17" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>156</v>
+      <c r="C18" s="26" t="s">
+        <v>125</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>23</v>
@@ -2783,22 +2794,22 @@
         <v>2019</v>
       </c>
       <c r="I18" s="13">
-        <v>7.13</v>
+        <v>7.05</v>
       </c>
       <c r="J18" s="13">
-        <v>55.65</v>
+        <v>42.43</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M18" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O18" s="13" t="s">
         <v>29</v>
@@ -2813,27 +2824,27 @@
         <v>32</v>
       </c>
       <c r="S18">
-        <v>1100000</v>
+        <v>400000</v>
       </c>
       <c r="T18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A19" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>159</v>
+      <c r="C19" s="26" t="s">
+        <v>128</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>23</v>
@@ -2845,10 +2856,10 @@
         <v>2019</v>
       </c>
       <c r="I19" s="13">
-        <v>8.0299999999999994</v>
+        <v>3.12</v>
       </c>
       <c r="J19" s="13">
-        <v>55.8</v>
+        <v>47.18</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>49</v>
@@ -2875,27 +2886,27 @@
         <v>32</v>
       </c>
       <c r="S19">
-        <v>700000</v>
+        <v>1200000</v>
       </c>
       <c r="T19" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>162</v>
+      <c r="C20" s="26" t="s">
+        <v>130</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>23</v>
@@ -2907,10 +2918,10 @@
         <v>2019</v>
       </c>
       <c r="I20" s="13">
-        <v>21.03</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>165</v>
+        <v>5.15</v>
+      </c>
+      <c r="J20" s="13">
+        <v>44.43</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>49</v>
@@ -2937,27 +2948,27 @@
         <v>32</v>
       </c>
       <c r="S20">
-        <v>100000</v>
-      </c>
-      <c r="T20">
-        <v>100</v>
+        <v>1500000</v>
+      </c>
+      <c r="T20" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>249</v>
+      <c r="C21" s="26" t="s">
+        <v>132</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>23</v>
@@ -2969,13 +2980,13 @@
         <v>2019</v>
       </c>
       <c r="I21" s="13">
-        <v>19.8</v>
+        <v>3.15</v>
       </c>
       <c r="J21" s="13">
-        <v>49.1</v>
+        <v>41.62</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>37</v>
@@ -2999,10 +3010,10 @@
         <v>32</v>
       </c>
       <c r="S21">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="T21" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:20" s="4" customFormat="1" ht="16">
@@ -3629,10 +3640,10 @@
       <c r="A32" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="25" t="s">
         <v>220</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -3691,10 +3702,10 @@
       <c r="A33" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="25" t="s">
         <v>221</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -3751,10 +3762,10 @@
       <c r="A34" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="25" t="s">
         <v>222</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -3809,10 +3820,10 @@
       <c r="A35" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="25" t="s">
         <v>223</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -4116,20 +4127,20 @@
       </c>
     </row>
     <row r="40" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A40" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>100</v>
+      <c r="A40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>23</v>
@@ -4141,10 +4152,10 @@
         <v>2019</v>
       </c>
       <c r="I40" s="13">
-        <v>9.25</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="J40" s="13">
-        <v>40.950000000000003</v>
+        <v>48.28</v>
       </c>
       <c r="K40" s="13" t="s">
         <v>49</v>
@@ -4162,7 +4173,7 @@
         <v>29</v>
       </c>
       <c r="P40" s="13" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="Q40" s="13" t="s">
         <v>31</v>
@@ -4171,27 +4182,27 @@
         <v>32</v>
       </c>
       <c r="S40">
-        <v>25000</v>
+        <v>45000</v>
       </c>
       <c r="T40">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A41" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>103</v>
+      <c r="A41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>23</v>
@@ -4203,10 +4214,10 @@
         <v>2019</v>
       </c>
       <c r="I41" s="13">
-        <v>3.63</v>
+        <v>5.53</v>
       </c>
       <c r="J41" s="13">
-        <v>118.7</v>
+        <v>71.3</v>
       </c>
       <c r="K41" s="13" t="s">
         <v>49</v>
@@ -4224,7 +4235,7 @@
         <v>29</v>
       </c>
       <c r="P41" s="13" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="Q41" s="13" t="s">
         <v>31</v>
@@ -4233,10 +4244,10 @@
         <v>32</v>
       </c>
       <c r="S41">
-        <v>20000</v>
+        <v>65000</v>
       </c>
       <c r="T41">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:20" s="4" customFormat="1" ht="16">
@@ -4247,13 +4258,13 @@
         <v>19</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>23</v>
@@ -4265,10 +4276,10 @@
         <v>2019</v>
       </c>
       <c r="I42" s="13">
-        <v>8.2200000000000006</v>
+        <v>7.45</v>
       </c>
       <c r="J42" s="13">
-        <v>48.28</v>
+        <v>60.93</v>
       </c>
       <c r="K42" s="13" t="s">
         <v>49</v>
@@ -4286,7 +4297,7 @@
         <v>29</v>
       </c>
       <c r="P42" s="13" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="Q42" s="13" t="s">
         <v>31</v>
@@ -4295,30 +4306,30 @@
         <v>32</v>
       </c>
       <c r="S42">
-        <v>45000</v>
+        <v>285000</v>
       </c>
       <c r="T42">
-        <v>45</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A43" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>105</v>
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>24</v>
@@ -4327,13 +4338,13 @@
         <v>2019</v>
       </c>
       <c r="I43" s="13">
-        <v>23.27</v>
+        <v>5.95</v>
       </c>
       <c r="J43" s="13">
-        <v>53.75</v>
+        <v>60.72</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="L43" s="13" t="s">
         <v>37</v>
@@ -4348,7 +4359,7 @@
         <v>29</v>
       </c>
       <c r="P43" s="13" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="Q43" s="13" t="s">
         <v>31</v>
@@ -4357,10 +4368,10 @@
         <v>32</v>
       </c>
       <c r="S43">
-        <v>80000</v>
+        <v>150000</v>
       </c>
       <c r="T43">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:20" s="4" customFormat="1" ht="16">
@@ -4371,13 +4382,13 @@
         <v>19</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>23</v>
@@ -4389,10 +4400,10 @@
         <v>2019</v>
       </c>
       <c r="I44" s="13">
-        <v>5.53</v>
+        <v>5.55</v>
       </c>
       <c r="J44" s="13">
-        <v>71.3</v>
+        <v>39.97</v>
       </c>
       <c r="K44" s="13" t="s">
         <v>49</v>
@@ -4410,7 +4421,7 @@
         <v>29</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Q44" s="13" t="s">
         <v>31</v>
@@ -4419,10 +4430,10 @@
         <v>32</v>
       </c>
       <c r="S44">
-        <v>65000</v>
+        <v>400000</v>
       </c>
       <c r="T44">
-        <v>65</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:20" s="4" customFormat="1" ht="16">
@@ -4433,35 +4444,33 @@
         <v>19</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="H45" s="13">
         <v>2019</v>
       </c>
       <c r="I45" s="13">
-        <v>7.45</v>
+        <v>25.42</v>
       </c>
       <c r="J45" s="13">
-        <v>60.93</v>
+        <v>53.82</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>37</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="L45" s="13"/>
       <c r="M45" s="13" t="s">
         <v>37</v>
       </c>
@@ -4472,7 +4481,7 @@
         <v>29</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="Q45" s="13" t="s">
         <v>31</v>
@@ -4481,30 +4490,30 @@
         <v>32</v>
       </c>
       <c r="S45">
-        <v>285000</v>
+        <v>180000</v>
       </c>
       <c r="T45">
-        <v>285</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>60</v>
+      <c r="A46" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>204</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>24</v>
@@ -4513,10 +4522,10 @@
         <v>2019</v>
       </c>
       <c r="I46" s="13">
-        <v>5.95</v>
+        <v>6.33</v>
       </c>
       <c r="J46" s="13">
-        <v>60.72</v>
+        <v>62.32</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>49</v>
@@ -4534,36 +4543,32 @@
         <v>29</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>58</v>
+        <v>205</v>
       </c>
       <c r="Q46" s="13" t="s">
-        <v>31</v>
+        <v>206</v>
       </c>
       <c r="R46" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S46">
-        <v>150000</v>
-      </c>
-      <c r="T46">
-        <v>150</v>
-      </c>
+      <c r="S46"/>
+      <c r="T46"/>
     </row>
     <row r="47" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A47" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>111</v>
+      <c r="A47" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>207</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>23</v>
@@ -4575,16 +4580,16 @@
         <v>2019</v>
       </c>
       <c r="I47" s="13">
-        <v>3.5</v>
+        <v>3.85</v>
       </c>
       <c r="J47" s="13">
-        <v>65.45</v>
+        <v>58.82</v>
       </c>
       <c r="K47" s="13" t="s">
         <v>49</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M47" s="13" t="s">
         <v>37</v>
@@ -4596,36 +4601,32 @@
         <v>29</v>
       </c>
       <c r="P47" s="13" t="s">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="Q47" s="13" t="s">
-        <v>31</v>
+        <v>206</v>
       </c>
       <c r="R47" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S47">
-        <v>220000</v>
-      </c>
-      <c r="T47">
-        <v>220</v>
-      </c>
+      <c r="S47"/>
+      <c r="T47"/>
     </row>
     <row r="48" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>63</v>
+      <c r="A48" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>183</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F48" s="13" t="s">
         <v>23</v>
@@ -4637,10 +4638,10 @@
         <v>2019</v>
       </c>
       <c r="I48" s="13">
-        <v>5.55</v>
+        <v>1.78</v>
       </c>
       <c r="J48" s="13">
-        <v>39.97</v>
+        <v>29.68</v>
       </c>
       <c r="K48" s="13" t="s">
         <v>49</v>
@@ -4658,56 +4659,54 @@
         <v>29</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="Q48" s="13" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="R48" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S48">
-        <v>400000</v>
-      </c>
-      <c r="T48">
-        <v>400</v>
-      </c>
+      <c r="S48"/>
+      <c r="T48"/>
     </row>
     <row r="49" spans="1:20" s="4" customFormat="1" ht="16">
-      <c r="A49" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>67</v>
+      <c r="A49" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="H49" s="13">
         <v>2019</v>
       </c>
       <c r="I49" s="13">
-        <v>25.42</v>
+        <v>2.65</v>
       </c>
       <c r="J49" s="13">
-        <v>53.82</v>
+        <v>34.520000000000003</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="L49" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="M49" s="13" t="s">
         <v>37</v>
       </c>
@@ -4718,33 +4717,29 @@
         <v>29</v>
       </c>
       <c r="P49" s="13" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="Q49" s="13" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="R49" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S49">
-        <v>180000</v>
-      </c>
-      <c r="T49">
-        <v>180</v>
-      </c>
+      <c r="S49"/>
+      <c r="T49"/>
     </row>
     <row r="50" spans="1:20" s="7" customFormat="1" ht="16">
       <c r="A50" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>197</v>
+      <c r="C50" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>193</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>194</v>
@@ -4759,29 +4754,31 @@
         <v>2019</v>
       </c>
       <c r="I50" s="13">
-        <v>21.12</v>
+        <v>6.58</v>
       </c>
       <c r="J50" s="13">
-        <v>35.630000000000003</v>
+        <v>45.2</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="L50" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="M50" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O50" s="13" t="s">
         <v>29</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Q50" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="R50" s="13" t="s">
         <v>32</v>
@@ -4793,154 +4790,158 @@
       <c r="A51" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C51" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>201</v>
+      <c r="C51" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>200</v>
       </c>
       <c r="E51" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I51" s="13">
+        <v>6.47</v>
+      </c>
+      <c r="J51" s="13">
+        <v>24.33</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O51" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P51" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q51" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="R51" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+    </row>
+    <row r="52" spans="1:20" s="14" customFormat="1" ht="16">
+      <c r="A52" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I52" s="13">
+        <v>11.08</v>
+      </c>
+      <c r="J52" s="13">
+        <v>38.479999999999997</v>
+      </c>
+      <c r="K52" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O52" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q52" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S52" s="32">
+        <v>80000</v>
+      </c>
+      <c r="T52" s="32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" s="14" customFormat="1" ht="16">
+      <c r="A53" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E53" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H51" s="13">
-        <v>2019</v>
-      </c>
-      <c r="I51" s="13">
-        <v>10.42</v>
-      </c>
-      <c r="J51" s="13">
-        <v>68.72</v>
-      </c>
-      <c r="K51" s="13" t="s">
+      <c r="F53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I53" s="13">
+        <v>8.58</v>
+      </c>
+      <c r="J53" s="13">
+        <v>45.35</v>
+      </c>
+      <c r="K53" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="L51" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M51" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="N51" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="O51" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="P51" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q51" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="R51" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S51"/>
-      <c r="T51"/>
-    </row>
-    <row r="52" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A52" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="E52" s="13">
-        <v>75</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="13">
-        <v>2019</v>
-      </c>
-      <c r="I52" s="13">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="J52" s="13">
-        <v>51.6</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="L52" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M52" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N52" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="O52" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="P52" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q52" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="R52" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S52"/>
-      <c r="T52"/>
-    </row>
-    <row r="53" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A53" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="13">
-        <v>2019</v>
-      </c>
-      <c r="I53" s="13">
-        <v>24.8</v>
-      </c>
-      <c r="J53" s="13">
-        <v>71.2</v>
-      </c>
-      <c r="K53" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="L53" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M53" s="13" t="s">
         <v>37</v>
@@ -4952,16 +4953,20 @@
         <v>29</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="Q53" s="13" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="R53" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S53"/>
-      <c r="T53"/>
+      <c r="S53" s="32">
+        <v>80000</v>
+      </c>
+      <c r="T53" s="32">
+        <v>80</v>
+      </c>
     </row>
     <row r="54" spans="1:20" s="14" customFormat="1" ht="16">
       <c r="A54" s="11" t="s">
@@ -4971,13 +4976,13 @@
         <v>232</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>23</v>
@@ -4989,28 +4994,28 @@
         <v>2019</v>
       </c>
       <c r="I54" s="13">
-        <v>6.78</v>
+        <v>5.2</v>
       </c>
       <c r="J54" s="13">
-        <v>69.55</v>
+        <v>84.07</v>
       </c>
       <c r="K54" s="13" t="s">
         <v>49</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M54" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N54" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O54" s="13" t="s">
         <v>29</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="Q54" s="13" t="s">
         <v>31</v>
@@ -5029,16 +5034,16 @@
         <v>232</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>24</v>
@@ -5047,31 +5052,29 @@
         <v>2019</v>
       </c>
       <c r="I55" s="13">
-        <v>5.4</v>
+        <v>21.12</v>
       </c>
       <c r="J55" s="13">
-        <v>106.2</v>
+        <v>35.630000000000003</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L55" s="13" t="s">
-        <v>36</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L55" s="13"/>
       <c r="M55" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N55" s="13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O55" s="13" t="s">
         <v>29</v>
       </c>
       <c r="P55" s="13" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="Q55" s="13" t="s">
-        <v>31</v>
+        <v>199</v>
       </c>
       <c r="R55" s="13" t="s">
         <v>32</v>
@@ -5087,13 +5090,13 @@
         <v>232</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="F56" s="13" t="s">
         <v>99</v>
@@ -5105,10 +5108,10 @@
         <v>2019</v>
       </c>
       <c r="I56" s="13">
-        <v>1.83</v>
+        <v>10.42</v>
       </c>
       <c r="J56" s="13">
-        <v>73.98</v>
+        <v>68.72</v>
       </c>
       <c r="K56" s="13" t="s">
         <v>49</v>
@@ -5126,10 +5129,10 @@
         <v>29</v>
       </c>
       <c r="P56" s="13" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="Q56" s="13" t="s">
-        <v>31</v>
+        <v>203</v>
       </c>
       <c r="R56" s="13" t="s">
         <v>32</v>
@@ -5138,20 +5141,20 @@
       <c r="T56"/>
     </row>
     <row r="57" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A57" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>174</v>
+      <c r="A57" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>23</v>
@@ -5163,15 +5166,17 @@
         <v>2019</v>
       </c>
       <c r="I57" s="13">
-        <v>16.32</v>
+        <v>9.25</v>
       </c>
       <c r="J57" s="13">
-        <v>107.95</v>
+        <v>40.950000000000003</v>
       </c>
       <c r="K57" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="L57" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="M57" s="13" t="s">
         <v>37</v>
       </c>
@@ -5182,7 +5187,7 @@
         <v>29</v>
       </c>
       <c r="P57" s="13" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="Q57" s="13" t="s">
         <v>31</v>
@@ -5190,45 +5195,49 @@
       <c r="R57" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S57"/>
-      <c r="T57"/>
+      <c r="S57">
+        <v>25000</v>
+      </c>
+      <c r="T57">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A58" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>177</v>
+      <c r="A58" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>103</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="F58" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="H58" s="13">
         <v>2019</v>
       </c>
       <c r="I58" s="13">
-        <v>22.47</v>
+        <v>3.63</v>
       </c>
       <c r="J58" s="13">
-        <v>119.07</v>
+        <v>118.7</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M58" s="13" t="s">
         <v>37</v>
@@ -5240,7 +5249,7 @@
         <v>29</v>
       </c>
       <c r="P58" s="13" t="s">
-        <v>179</v>
+        <v>102</v>
       </c>
       <c r="Q58" s="13" t="s">
         <v>31</v>
@@ -5248,27 +5257,31 @@
       <c r="R58" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S58"/>
-      <c r="T58"/>
+      <c r="S58">
+        <v>20000</v>
+      </c>
+      <c r="T58">
+        <v>20</v>
+      </c>
     </row>
     <row r="59" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A59" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>180</v>
+      <c r="A59" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>105</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>24</v>
@@ -5277,28 +5290,28 @@
         <v>2019</v>
       </c>
       <c r="I59" s="13">
-        <v>5.2</v>
+        <v>23.27</v>
       </c>
       <c r="J59" s="13">
-        <v>84.07</v>
+        <v>53.75</v>
       </c>
       <c r="K59" s="13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M59" s="13" t="s">
         <v>37</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O59" s="13" t="s">
         <v>29</v>
       </c>
       <c r="P59" s="13" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
       <c r="Q59" s="13" t="s">
         <v>31</v>
@@ -5306,27 +5319,31 @@
       <c r="R59" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S59"/>
-      <c r="T59"/>
+      <c r="S59">
+        <v>80000</v>
+      </c>
+      <c r="T59">
+        <v>80</v>
+      </c>
     </row>
     <row r="60" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A60" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>204</v>
+      <c r="A60" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>111</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>24</v>
@@ -5335,10 +5352,10 @@
         <v>2019</v>
       </c>
       <c r="I60" s="13">
-        <v>6.33</v>
+        <v>3.5</v>
       </c>
       <c r="J60" s="13">
-        <v>62.32</v>
+        <v>65.45</v>
       </c>
       <c r="K60" s="13" t="s">
         <v>49</v>
@@ -5356,16 +5373,20 @@
         <v>29</v>
       </c>
       <c r="P60" s="13" t="s">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="Q60" s="13" t="s">
-        <v>206</v>
+        <v>31</v>
       </c>
       <c r="R60" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S60"/>
-      <c r="T60"/>
+      <c r="S60">
+        <v>220000</v>
+      </c>
+      <c r="T60">
+        <v>220</v>
+      </c>
     </row>
     <row r="61" spans="1:20" s="14" customFormat="1" ht="16">
       <c r="A61" s="11" t="s">
@@ -5375,16 +5396,16 @@
         <v>232</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>208</v>
+        <v>189</v>
+      </c>
+      <c r="E61" s="13">
+        <v>75</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>24</v>
@@ -5393,19 +5414,19 @@
         <v>2019</v>
       </c>
       <c r="I61" s="13">
-        <v>3.85</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="J61" s="13">
-        <v>58.82</v>
+        <v>51.6</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N61" s="13" t="s">
         <v>38</v>
@@ -5414,10 +5435,10 @@
         <v>29</v>
       </c>
       <c r="P61" s="13" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="Q61" s="13" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="R61" s="13" t="s">
         <v>32</v>
@@ -5433,16 +5454,16 @@
         <v>232</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>24</v>
@@ -5451,16 +5472,16 @@
         <v>2019</v>
       </c>
       <c r="I62" s="13">
-        <v>1.78</v>
+        <v>24.8</v>
       </c>
       <c r="J62" s="13">
-        <v>29.68</v>
+        <v>71.2</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L62" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M62" s="13" t="s">
         <v>37</v>
@@ -5472,10 +5493,10 @@
         <v>29</v>
       </c>
       <c r="P62" s="13" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="Q62" s="13" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="R62" s="13" t="s">
         <v>32</v>
@@ -5491,16 +5512,16 @@
         <v>232</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>170</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>24</v>
@@ -5509,10 +5530,10 @@
         <v>2019</v>
       </c>
       <c r="I63" s="13">
-        <v>2.65</v>
+        <v>6.78</v>
       </c>
       <c r="J63" s="13">
-        <v>34.520000000000003</v>
+        <v>69.55</v>
       </c>
       <c r="K63" s="13" t="s">
         <v>49</v>
@@ -5530,10 +5551,10 @@
         <v>29</v>
       </c>
       <c r="P63" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="Q63" s="13" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="R63" s="13" t="s">
         <v>32</v>
@@ -5549,16 +5570,16 @@
         <v>232</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>193</v>
+        <v>235</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>172</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>24</v>
@@ -5567,10 +5588,10 @@
         <v>2019</v>
       </c>
       <c r="I64" s="13">
-        <v>6.58</v>
+        <v>5.4</v>
       </c>
       <c r="J64" s="13">
-        <v>45.2</v>
+        <v>106.2</v>
       </c>
       <c r="K64" s="13" t="s">
         <v>25</v>
@@ -5588,10 +5609,10 @@
         <v>29</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="Q64" s="13" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="R64" s="13" t="s">
         <v>32</v>
@@ -5607,13 +5628,13 @@
         <v>232</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>23</v>
@@ -5625,17 +5646,15 @@
         <v>2019</v>
       </c>
       <c r="I65" s="13">
-        <v>6.47</v>
+        <v>16.32</v>
       </c>
       <c r="J65" s="13">
-        <v>24.33</v>
+        <v>107.95</v>
       </c>
       <c r="K65" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L65" s="13" t="s">
-        <v>37</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L65" s="13"/>
       <c r="M65" s="13" t="s">
         <v>37</v>
       </c>
@@ -5646,53 +5665,53 @@
         <v>29</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="Q65" s="13" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="R65" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
+      <c r="S65"/>
+      <c r="T65"/>
     </row>
     <row r="66" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A66" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>107</v>
+      <c r="A66" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>177</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="F66" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H66" s="13">
         <v>2019</v>
       </c>
       <c r="I66" s="13">
-        <v>11.08</v>
+        <v>22.47</v>
       </c>
       <c r="J66" s="13">
-        <v>38.479999999999997</v>
+        <v>119.07</v>
       </c>
       <c r="K66" s="13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L66" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M66" s="13" t="s">
         <v>37</v>
@@ -5704,39 +5723,35 @@
         <v>29</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>108</v>
+        <v>179</v>
       </c>
       <c r="Q66" s="13" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="R66" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S66" s="33">
-        <v>80000</v>
-      </c>
-      <c r="T66" s="33">
-        <v>80</v>
-      </c>
+      <c r="S66"/>
+      <c r="T66"/>
     </row>
     <row r="67" spans="1:20" s="14" customFormat="1" ht="16">
-      <c r="A67" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>110</v>
+      <c r="A67" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>173</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>24</v>
@@ -5745,10 +5760,10 @@
         <v>2019</v>
       </c>
       <c r="I67" s="13">
-        <v>8.58</v>
+        <v>1.83</v>
       </c>
       <c r="J67" s="13">
-        <v>45.35</v>
+        <v>73.98</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>49</v>
@@ -5766,32 +5781,28 @@
         <v>29</v>
       </c>
       <c r="P67" s="13" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="Q67" s="13" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="R67" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S67" s="33">
-        <v>80000</v>
-      </c>
-      <c r="T67" s="33">
-        <v>80</v>
-      </c>
+      <c r="S67"/>
+      <c r="T67"/>
     </row>
     <row r="68" spans="1:20" ht="16">
       <c r="A68" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="29" t="s">
         <v>310</v>
       </c>
       <c r="E68" s="13" t="s">
@@ -5839,13 +5850,13 @@
       <c r="A69" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C69" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="D69" s="30" t="s">
+      <c r="D69" s="29" t="s">
         <v>311</v>
       </c>
       <c r="E69" s="13" t="s">
@@ -5895,13 +5906,13 @@
       <c r="A70" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C70" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="29" t="s">
         <v>312</v>
       </c>
       <c r="E70" s="13" t="s">
@@ -5951,13 +5962,13 @@
       <c r="A71" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C71" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="D71" s="30" t="s">
+      <c r="D71" s="29" t="s">
         <v>313</v>
       </c>
       <c r="E71" s="13" t="s">
@@ -6007,55 +6018,55 @@
       <c r="A72" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="C72" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="D72" s="30" t="s">
+      <c r="D72" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="F72" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G72" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H72" s="20">
-        <v>2019</v>
-      </c>
-      <c r="I72" s="20">
+      <c r="F72" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" s="19">
+        <v>2019</v>
+      </c>
+      <c r="I72" s="19">
         <v>5.28</v>
       </c>
-      <c r="J72" s="20">
+      <c r="J72" s="19">
         <v>47.93</v>
       </c>
-      <c r="K72" s="20" t="s">
+      <c r="K72" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="L72" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="M72" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="N72" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="O72" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P72" s="20" t="s">
+      <c r="L72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N72" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O72" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="P72" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="Q72" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="R72" s="20" t="s">
+      <c r="Q72" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="R72" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6063,55 +6074,55 @@
       <c r="A73" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C73" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="D73" s="30" t="s">
+      <c r="D73" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="E73" s="21" t="s">
+      <c r="E73" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="F73" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G73" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H73" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I73" s="21">
+      <c r="F73" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I73" s="20">
         <v>7.78</v>
       </c>
-      <c r="J73" s="21">
+      <c r="J73" s="20">
         <v>45.48</v>
       </c>
-      <c r="K73" s="21" t="s">
+      <c r="K73" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L73" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M73" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N73" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O73" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P73" s="21" t="s">
+      <c r="L73" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M73" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N73" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O73" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P73" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q73" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R73" s="21" t="s">
+      <c r="Q73" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R73" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6119,55 +6130,55 @@
       <c r="A74" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C74" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F74" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G74" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H74" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I74" s="21">
+      <c r="F74" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H74" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I74" s="20">
         <v>5.77</v>
       </c>
-      <c r="J74" s="21">
+      <c r="J74" s="20">
         <v>47.27</v>
       </c>
-      <c r="K74" s="21" t="s">
+      <c r="K74" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L74" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M74" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N74" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O74" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P74" s="21" t="s">
+      <c r="L74" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N74" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O74" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q74" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R74" s="21" t="s">
+      <c r="Q74" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R74" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6175,55 +6186,55 @@
       <c r="A75" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="D75" s="30" t="s">
+      <c r="D75" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="E75" s="21" t="s">
+      <c r="E75" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="F75" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G75" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H75" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I75" s="21">
+      <c r="F75" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H75" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I75" s="20">
         <v>4.83</v>
       </c>
-      <c r="J75" s="21">
+      <c r="J75" s="20">
         <v>48.22</v>
       </c>
-      <c r="K75" s="21" t="s">
+      <c r="K75" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L75" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M75" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N75" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O75" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P75" s="21" t="s">
+      <c r="L75" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M75" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N75" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O75" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q75" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R75" s="21" t="s">
+      <c r="Q75" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R75" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6231,53 +6242,53 @@
       <c r="A76" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="D76" s="30" t="s">
+      <c r="D76" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="E76" s="21" t="s">
+      <c r="E76" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="F76" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G76" s="21" t="s">
+      <c r="F76" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G76" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="H76" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I76" s="21">
+      <c r="H76" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I76" s="20">
         <v>26.28</v>
       </c>
-      <c r="J76" s="21">
+      <c r="J76" s="20">
         <v>54.15</v>
       </c>
-      <c r="K76" s="21" t="s">
+      <c r="K76" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L76" s="21"/>
-      <c r="M76" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N76" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O76" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P76" s="21" t="s">
+      <c r="L76" s="20"/>
+      <c r="M76" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N76" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O76" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P76" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q76" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R76" s="21" t="s">
+      <c r="Q76" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R76" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6285,53 +6296,53 @@
       <c r="A77" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D77" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="E77" s="21" t="s">
+      <c r="E77" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="F77" s="21" t="s">
+      <c r="F77" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="G77" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H77" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I77" s="21">
+      <c r="G77" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H77" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I77" s="20">
         <v>3.65</v>
       </c>
-      <c r="J77" s="21">
+      <c r="J77" s="20">
         <v>47.25</v>
       </c>
-      <c r="K77" s="21" t="s">
+      <c r="K77" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L77" s="21"/>
-      <c r="M77" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N77" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O77" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P77" s="21" t="s">
+      <c r="L77" s="20"/>
+      <c r="M77" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N77" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O77" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q77" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R77" s="21" t="s">
+      <c r="Q77" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R77" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6339,55 +6350,55 @@
       <c r="A78" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="D78" s="30" t="s">
+      <c r="D78" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="E78" s="21" t="s">
+      <c r="E78" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F78" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G78" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H78" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I78" s="21">
+      <c r="F78" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I78" s="20">
         <v>7.97</v>
       </c>
-      <c r="J78" s="21">
+      <c r="J78" s="20">
         <v>42.15</v>
       </c>
-      <c r="K78" s="21" t="s">
+      <c r="K78" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L78" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M78" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N78" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O78" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P78" s="21" t="s">
+      <c r="L78" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M78" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N78" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O78" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q78" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R78" s="21" t="s">
+      <c r="Q78" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R78" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6395,55 +6406,55 @@
       <c r="A79" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D79" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="E79" s="21" t="s">
+      <c r="E79" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F79" s="21" t="s">
+      <c r="F79" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="G79" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H79" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I79" s="21">
+      <c r="G79" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I79" s="20">
         <v>6.75</v>
       </c>
-      <c r="J79" s="21">
+      <c r="J79" s="20">
         <v>65.400000000000006</v>
       </c>
-      <c r="K79" s="21" t="s">
+      <c r="K79" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N79" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O79" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P79" s="21" t="s">
+      <c r="L79" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M79" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N79" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O79" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q79" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R79" s="21" t="s">
+      <c r="Q79" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R79" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6451,55 +6462,55 @@
       <c r="A80" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D80" s="18" t="s">
+      <c r="D80" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="E80" s="21" t="s">
+      <c r="E80" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="F80" s="21" t="s">
+      <c r="F80" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="G80" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H80" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I80" s="21">
+      <c r="G80" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I80" s="20">
         <v>3.75</v>
       </c>
-      <c r="J80" s="21">
+      <c r="J80" s="20">
         <v>68.17</v>
       </c>
-      <c r="K80" s="21" t="s">
+      <c r="K80" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L80" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M80" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N80" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O80" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P80" s="21" t="s">
+      <c r="L80" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M80" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N80" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O80" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P80" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q80" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R80" s="21" t="s">
+      <c r="Q80" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R80" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6507,55 +6518,55 @@
       <c r="A81" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C81" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="D81" s="18" t="s">
+      <c r="D81" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="E81" s="21" t="s">
+      <c r="E81" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F81" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G81" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H81" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I81" s="21">
+      <c r="F81" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I81" s="20">
         <v>4.47</v>
       </c>
-      <c r="J81" s="21">
+      <c r="J81" s="20">
         <v>43.92</v>
       </c>
-      <c r="K81" s="21" t="s">
+      <c r="K81" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L81" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M81" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N81" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O81" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P81" s="21" t="s">
+      <c r="L81" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M81" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N81" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O81" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q81" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R81" s="21" t="s">
+      <c r="Q81" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R81" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6563,13 +6574,13 @@
       <c r="A82" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="D82" s="32" t="s">
+      <c r="D82" s="31" t="s">
         <v>274</v>
       </c>
       <c r="E82" s="13" t="s">
@@ -6619,13 +6630,13 @@
       <c r="A83" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="D83" s="32" t="s">
+      <c r="D83" s="31" t="s">
         <v>275</v>
       </c>
       <c r="E83" s="13" t="s">
@@ -6675,13 +6686,13 @@
       <c r="A84" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C84" s="17" t="s">
+      <c r="C84" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="D84" s="32" t="s">
+      <c r="D84" s="31" t="s">
         <v>276</v>
       </c>
       <c r="E84" s="13" t="s">
@@ -6729,13 +6740,13 @@
       <c r="A85" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C85" s="17" t="s">
+      <c r="C85" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="D85" s="32" t="s">
+      <c r="D85" s="31" t="s">
         <v>277</v>
       </c>
       <c r="E85" s="13" t="s">
@@ -6783,13 +6794,13 @@
       <c r="A86" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C86" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D86" s="17" t="s">
         <v>278</v>
       </c>
       <c r="E86" s="13" t="s">
@@ -6839,55 +6850,55 @@
       <c r="A87" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C87" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="D87" s="18" t="s">
+      <c r="D87" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E87" s="21" t="s">
+      <c r="E87" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F87" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G87" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H87" s="21">
-        <v>2019</v>
-      </c>
-      <c r="I87" s="21">
+      <c r="F87" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G87" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I87" s="20">
         <v>5.0199999999999996</v>
       </c>
-      <c r="J87" s="21">
+      <c r="J87" s="20">
         <v>50.57</v>
       </c>
-      <c r="K87" s="21" t="s">
+      <c r="K87" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L87" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M87" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N87" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O87" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P87" s="21" t="s">
+      <c r="L87" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M87" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N87" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O87" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q87" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R87" s="21" t="s">
+      <c r="Q87" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R87" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6895,13 +6906,13 @@
       <c r="A88" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C88" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D88" s="31" t="s">
+      <c r="D88" s="30" t="s">
         <v>280</v>
       </c>
       <c r="E88" s="13" t="s">
@@ -6951,13 +6962,13 @@
       <c r="A89" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D89" s="31" t="s">
+      <c r="D89" s="30" t="s">
         <v>281</v>
       </c>
       <c r="E89" s="13" t="s">
@@ -7007,13 +7018,13 @@
       <c r="A90" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="D90" s="31" t="s">
+      <c r="D90" s="30" t="s">
         <v>282</v>
       </c>
       <c r="E90" s="13" t="s">
@@ -7063,13 +7074,13 @@
       <c r="A91" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="D91" s="31" t="s">
+      <c r="D91" s="30" t="s">
         <v>283</v>
       </c>
       <c r="E91" s="13" t="s">
@@ -7119,13 +7130,13 @@
       <c r="A92" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D92" s="31" t="s">
+      <c r="D92" s="30" t="s">
         <v>284</v>
       </c>
       <c r="E92" s="13" t="s">
@@ -7175,20 +7186,20 @@
       <c r="A93" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C93" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="D93" s="32" t="s">
-        <v>290</v>
+      <c r="C93" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>285</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>296</v>
+        <v>85</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>24</v>
@@ -7197,16 +7208,16 @@
         <v>2019</v>
       </c>
       <c r="I93" s="13">
-        <v>7.73</v>
+        <v>22.55</v>
       </c>
       <c r="J93" s="13">
-        <v>43.23</v>
+        <v>51.5</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L93" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M93" s="13" t="s">
         <v>37</v>
@@ -7231,17 +7242,17 @@
       <c r="A94" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C94" s="17" t="s">
-        <v>269</v>
-      </c>
-      <c r="D94" s="32" t="s">
-        <v>289</v>
+      <c r="C94" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>286</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="F94" s="13" t="s">
         <v>23</v>
@@ -7253,10 +7264,10 @@
         <v>2019</v>
       </c>
       <c r="I94" s="13">
-        <v>2.82</v>
+        <v>4.62</v>
       </c>
       <c r="J94" s="13">
-        <v>47.68</v>
+        <v>41.27</v>
       </c>
       <c r="K94" s="13" t="s">
         <v>49</v>
@@ -7287,17 +7298,17 @@
       <c r="A95" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C95" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>288</v>
+      <c r="C95" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>287</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="F95" s="13" t="s">
         <v>23</v>
@@ -7309,10 +7320,10 @@
         <v>2019</v>
       </c>
       <c r="I95" s="13">
-        <v>9.67</v>
+        <v>6.2</v>
       </c>
       <c r="J95" s="13">
-        <v>40.28</v>
+        <v>42.98</v>
       </c>
       <c r="K95" s="13" t="s">
         <v>49</v>
@@ -7343,17 +7354,17 @@
       <c r="A96" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C96" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>287</v>
+      <c r="C96" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>288</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="F96" s="13" t="s">
         <v>23</v>
@@ -7365,10 +7376,10 @@
         <v>2019</v>
       </c>
       <c r="I96" s="13">
-        <v>6.2</v>
+        <v>9.67</v>
       </c>
       <c r="J96" s="13">
-        <v>42.98</v>
+        <v>40.28</v>
       </c>
       <c r="K96" s="13" t="s">
         <v>49</v>
@@ -7399,17 +7410,17 @@
       <c r="A97" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C97" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="D97" s="22" t="s">
-        <v>286</v>
+      <c r="C97" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D97" s="31" t="s">
+        <v>289</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>297</v>
+        <v>158</v>
       </c>
       <c r="F97" s="13" t="s">
         <v>23</v>
@@ -7421,10 +7432,10 @@
         <v>2019</v>
       </c>
       <c r="I97" s="13">
-        <v>4.62</v>
+        <v>2.82</v>
       </c>
       <c r="J97" s="13">
-        <v>41.27</v>
+        <v>47.68</v>
       </c>
       <c r="K97" s="13" t="s">
         <v>49</v>
@@ -7455,20 +7466,20 @@
       <c r="A98" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C98" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="D98" s="22" t="s">
-        <v>285</v>
+      <c r="C98" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>290</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>85</v>
+        <v>296</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>24</v>
@@ -7477,16 +7488,16 @@
         <v>2019</v>
       </c>
       <c r="I98" s="13">
-        <v>22.55</v>
+        <v>7.73</v>
       </c>
       <c r="J98" s="13">
-        <v>51.5</v>
+        <v>43.23</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M98" s="13" t="s">
         <v>37</v>
@@ -7508,9 +7519,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R98" xr:uid="{B89CD138-8E45-AB4F-9192-FF139BFA344F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R94">
-      <sortCondition ref="D1:D94"/>
+  <autoFilter ref="A1:T98" xr:uid="{CF3E64C5-3E35-4D4B-9072-3C01CE9577D9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T98">
+      <sortCondition ref="C1:C98"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
additional urine sample analysis
</commit_message>
<xml_diff>
--- a/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
+++ b/arup_urine_samples_ge_study/ge_distribution/190904_Urine_Sample_Processing_Log.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmontgomery/OneDrive/Documents/IDbyDNA/Code/AbsoluteQuantification/arup_urine_samples_ge_study/ge_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8217E1F2-606F-4847-8843-DD155BA7450F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39AB99A-34D4-404F-A4AB-FD567EE538B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="43160" windowHeight="20540" xr2:uid="{03398125-E31F-8D40-8D2D-1CD76C452301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample Log'!$A$1:$T$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample Log'!$A$1:$U$98</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="363">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -1084,12 +1084,81 @@
   <si>
     <t>21 confluent streaks</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Repeated as IDBD-D100509. Negative on repeat</t>
+  </si>
+  <si>
+    <t>Repeated as IDBD-D100510. Negative on repeat</t>
+  </si>
+  <si>
+    <t>Repeated as IDBD-D100511. Negative on repeat. Below cutoff.</t>
+  </si>
+  <si>
+    <t>Repeated as IDBD-D100513. Negative on repeat.</t>
+  </si>
+  <si>
+    <t>Repeated as IDBD-D100514. Negative on repeat. Just below cutoff by 3.2%.</t>
+  </si>
+  <si>
+    <t>190910B01</t>
+  </si>
+  <si>
+    <t>190913-1-1</t>
+  </si>
+  <si>
+    <t>IDBD-D100509</t>
+  </si>
+  <si>
+    <t>IDBD-D100510</t>
+  </si>
+  <si>
+    <t>IDBD-D100511</t>
+  </si>
+  <si>
+    <t>IDBD-D100512</t>
+  </si>
+  <si>
+    <t>IDBD-D100513</t>
+  </si>
+  <si>
+    <t>IDBD-D100514</t>
+  </si>
+  <si>
+    <t>IDBD-D100492</t>
+  </si>
+  <si>
+    <t>IDbyDNA-5478</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100414</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100415</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100416</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100420</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100440</t>
+  </si>
+  <si>
+    <t>Repeat of IDBD-D100441</t>
+  </si>
+  <si>
+    <t>The "RESULT LONG TEXT" column entry is an educated guess.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1157,6 +1226,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1207,7 +1301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1297,11 +1391,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1384,6 +1487,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,13 +1810,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38306794-63FA-0746-9C8B-867300C82BA0}">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:AF1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B68" workbookViewId="0">
+      <selection activeCell="P110" sqref="P110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.5" style="8"/>
     <col min="3" max="3" width="18.1640625" style="8" customWidth="1"/>
@@ -1719,7 +1831,7 @@
     <col min="21" max="16384" width="11.5" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="44" customHeight="1">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="44" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1780,8 +1892,11 @@
       <c r="T1" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1">
+      <c r="U1" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A2" s="4" t="s">
         <v>113</v>
       </c>
@@ -1843,7 +1958,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="4" customFormat="1">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A3" s="4" t="s">
         <v>113</v>
       </c>
@@ -1905,7 +2020,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="4" customFormat="1">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
@@ -1967,7 +2082,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="4" customFormat="1">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A5" s="4" t="s">
         <v>113</v>
       </c>
@@ -2029,7 +2144,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="4" customFormat="1">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -2091,7 +2206,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="4" customFormat="1">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
@@ -2153,7 +2268,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="4" customFormat="1">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A8" s="4" t="s">
         <v>113</v>
       </c>
@@ -2215,7 +2330,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="4" customFormat="1">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
@@ -2277,7 +2392,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="4" customFormat="1">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
@@ -2339,7 +2454,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="4" customFormat="1">
+    <row r="11" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A11" s="4" t="s">
         <v>113</v>
       </c>
@@ -2401,7 +2516,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="4" customFormat="1">
+    <row r="12" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A12" s="4" t="s">
         <v>113</v>
       </c>
@@ -2463,7 +2578,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="4" customFormat="1">
+    <row r="13" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A13" s="4" t="s">
         <v>113</v>
       </c>
@@ -2523,7 +2638,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="4" customFormat="1">
+    <row r="14" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A14" s="4" t="s">
         <v>113</v>
       </c>
@@ -2585,7 +2700,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="4" customFormat="1">
+    <row r="15" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A15" s="4" t="s">
         <v>113</v>
       </c>
@@ -2647,7 +2762,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="4" customFormat="1">
+    <row r="16" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A16" s="4" t="s">
         <v>113</v>
       </c>
@@ -2707,7 +2822,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="4" customFormat="1">
+    <row r="17" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A17" s="4" t="s">
         <v>113</v>
       </c>
@@ -2769,7 +2884,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="4" customFormat="1">
+    <row r="18" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A18" s="4" t="s">
         <v>113</v>
       </c>
@@ -2831,7 +2946,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="4" customFormat="1">
+    <row r="19" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A19" s="4" t="s">
         <v>113</v>
       </c>
@@ -2893,7 +3008,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="4" customFormat="1">
+    <row r="20" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
@@ -2955,7 +3070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="4" customFormat="1">
+    <row r="21" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A21" s="4" t="s">
         <v>113</v>
       </c>
@@ -3017,7 +3132,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="4" customFormat="1">
+    <row r="22" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A22" s="9" t="s">
         <v>230</v>
       </c>
@@ -3079,7 +3194,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="4" customFormat="1">
+    <row r="23" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A23" s="9" t="s">
         <v>230</v>
       </c>
@@ -3141,7 +3256,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="4" customFormat="1">
+    <row r="24" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A24" s="9" t="s">
         <v>230</v>
       </c>
@@ -3203,7 +3318,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="4" customFormat="1">
+    <row r="25" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A25" s="9" t="s">
         <v>230</v>
       </c>
@@ -3265,7 +3380,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="4" customFormat="1">
+    <row r="26" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A26" s="9" t="s">
         <v>230</v>
       </c>
@@ -3327,7 +3442,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="4" customFormat="1">
+    <row r="27" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A27" s="9" t="s">
         <v>230</v>
       </c>
@@ -3389,7 +3504,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="4" customFormat="1">
+    <row r="28" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A28" s="9" t="s">
         <v>230</v>
       </c>
@@ -3451,7 +3566,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="4" customFormat="1">
+    <row r="29" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A29" s="9" t="s">
         <v>230</v>
       </c>
@@ -3513,7 +3628,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="4" customFormat="1">
+    <row r="30" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A30" s="9" t="s">
         <v>230</v>
       </c>
@@ -3575,7 +3690,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="4" customFormat="1">
+    <row r="31" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A31" s="9" t="s">
         <v>230</v>
       </c>
@@ -3637,7 +3752,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="4" customFormat="1">
+    <row r="32" spans="1:20" s="4" customFormat="1" ht="16">
       <c r="A32" s="9" t="s">
         <v>230</v>
       </c>
@@ -3699,7 +3814,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="4" customFormat="1">
+    <row r="33" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A33" s="9" t="s">
         <v>230</v>
       </c>
@@ -3759,7 +3874,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="4" customFormat="1">
+    <row r="34" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A34" s="9" t="s">
         <v>230</v>
       </c>
@@ -3817,7 +3932,7 @@
       <c r="S34" s="35"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="1:20" s="4" customFormat="1">
+    <row r="35" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A35" s="9" t="s">
         <v>230</v>
       </c>
@@ -3879,7 +3994,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="4" customFormat="1">
+    <row r="36" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
@@ -3941,7 +4056,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="4" customFormat="1">
+    <row r="37" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A37" s="2" t="s">
         <v>18</v>
       </c>
@@ -4003,7 +4118,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="4" customFormat="1">
+    <row r="38" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
@@ -4065,7 +4180,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="4" customFormat="1">
+    <row r="39" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -4126,8 +4241,11 @@
       <c r="T39">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" s="4" customFormat="1">
+      <c r="U39" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A40" s="9" t="s">
         <v>230</v>
       </c>
@@ -4189,7 +4307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="4" customFormat="1">
+    <row r="41" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A41" s="9" t="s">
         <v>230</v>
       </c>
@@ -4251,7 +4369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="4" customFormat="1">
+    <row r="42" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -4312,8 +4430,11 @@
       <c r="T42">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" s="4" customFormat="1">
+      <c r="U42" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A43" s="9" t="s">
         <v>230</v>
       </c>
@@ -4375,7 +4496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="4" customFormat="1">
+    <row r="44" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -4436,8 +4557,11 @@
       <c r="T44">
         <v>65</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" s="4" customFormat="1">
+      <c r="U44" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -4499,7 +4623,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="4" customFormat="1">
+    <row r="46" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -4561,7 +4685,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="4" customFormat="1">
+    <row r="47" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A47" s="9" t="s">
         <v>230</v>
       </c>
@@ -4623,7 +4747,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="4" customFormat="1">
+    <row r="48" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
@@ -4685,7 +4809,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="4" customFormat="1">
+    <row r="49" spans="1:21" s="4" customFormat="1" ht="16">
       <c r="A49" s="2" t="s">
         <v>18</v>
       </c>
@@ -4745,7 +4869,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="7" customFormat="1">
+    <row r="50" spans="1:21" s="7" customFormat="1" ht="16">
       <c r="A50" s="11" t="s">
         <v>231</v>
       </c>
@@ -4803,7 +4927,7 @@
       </c>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" s="7" customFormat="1">
+    <row r="51" spans="1:21" s="7" customFormat="1" ht="16">
       <c r="A51" s="11" t="s">
         <v>231</v>
       </c>
@@ -4861,7 +4985,7 @@
       <c r="S51" s="32"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="14" customFormat="1">
+    <row r="52" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A52" s="11" t="s">
         <v>231</v>
       </c>
@@ -4919,7 +5043,7 @@
       <c r="S52" s="32"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="14" customFormat="1">
+    <row r="53" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A53" s="11" t="s">
         <v>231</v>
       </c>
@@ -4979,7 +5103,7 @@
       </c>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="14" customFormat="1">
+    <row r="54" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A54" s="11" t="s">
         <v>231</v>
       </c>
@@ -5039,7 +5163,7 @@
       </c>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="14" customFormat="1">
+    <row r="55" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A55" s="11" t="s">
         <v>231</v>
       </c>
@@ -5099,7 +5223,7 @@
       </c>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="14" customFormat="1">
+    <row r="56" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A56" s="11" t="s">
         <v>231</v>
       </c>
@@ -5159,7 +5283,7 @@
       </c>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="14" customFormat="1">
+    <row r="57" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A57" s="11" t="s">
         <v>231</v>
       </c>
@@ -5217,7 +5341,7 @@
       </c>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="14" customFormat="1">
+    <row r="58" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A58" s="11" t="s">
         <v>231</v>
       </c>
@@ -5277,7 +5401,7 @@
       </c>
       <c r="T58"/>
     </row>
-    <row r="59" spans="1:20" s="14" customFormat="1">
+    <row r="59" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A59" s="11" t="s">
         <v>231</v>
       </c>
@@ -5337,7 +5461,7 @@
       </c>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="14" customFormat="1">
+    <row r="60" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A60" s="11" t="s">
         <v>231</v>
       </c>
@@ -5397,7 +5521,7 @@
       </c>
       <c r="T60"/>
     </row>
-    <row r="61" spans="1:20" s="14" customFormat="1">
+    <row r="61" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A61" s="11" t="s">
         <v>231</v>
       </c>
@@ -5457,7 +5581,7 @@
       </c>
       <c r="T61"/>
     </row>
-    <row r="62" spans="1:20" s="14" customFormat="1">
+    <row r="62" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A62" s="11" t="s">
         <v>231</v>
       </c>
@@ -5516,8 +5640,11 @@
         <v>60000</v>
       </c>
       <c r="T62"/>
-    </row>
-    <row r="63" spans="1:20" s="14" customFormat="1">
+      <c r="U62" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A63" s="11" t="s">
         <v>231</v>
       </c>
@@ -5574,8 +5701,11 @@
       </c>
       <c r="S63" s="35"/>
       <c r="T63"/>
-    </row>
-    <row r="64" spans="1:20" s="14" customFormat="1">
+      <c r="U63" s="14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" s="14" customFormat="1" ht="16">
       <c r="A64" s="11" t="s">
         <v>231</v>
       </c>
@@ -5633,7 +5763,7 @@
       <c r="S64" s="35"/>
       <c r="T64"/>
     </row>
-    <row r="65" spans="1:20" s="14" customFormat="1">
+    <row r="65" spans="1:20" s="14" customFormat="1" ht="16">
       <c r="A65" s="11" t="s">
         <v>231</v>
       </c>
@@ -5693,7 +5823,7 @@
       </c>
       <c r="T65" s="4"/>
     </row>
-    <row r="66" spans="1:20" s="14" customFormat="1">
+    <row r="66" spans="1:20" s="14" customFormat="1" ht="16">
       <c r="A66" s="9" t="s">
         <v>230</v>
       </c>
@@ -5755,7 +5885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:20" s="14" customFormat="1">
+    <row r="67" spans="1:20" s="14" customFormat="1" ht="16">
       <c r="A67" s="9" t="s">
         <v>230</v>
       </c>
@@ -5817,7 +5947,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" ht="16">
       <c r="A68" s="8" t="s">
         <v>321</v>
       </c>
@@ -5874,7 +6004,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" ht="16">
       <c r="A69" s="8" t="s">
         <v>321</v>
       </c>
@@ -5933,7 +6063,7 @@
         <v>1300000</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" ht="16">
       <c r="A70" s="8" t="s">
         <v>321</v>
       </c>
@@ -5992,7 +6122,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" ht="16">
       <c r="A71" s="8" t="s">
         <v>321</v>
       </c>
@@ -6051,7 +6181,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" ht="16">
       <c r="A72" s="8" t="s">
         <v>321</v>
       </c>
@@ -6110,7 +6240,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" ht="16">
       <c r="A73" s="8" t="s">
         <v>321</v>
       </c>
@@ -6169,7 +6299,7 @@
         <v>1900000</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" ht="16">
       <c r="A74" s="8" t="s">
         <v>321</v>
       </c>
@@ -6228,7 +6358,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" ht="16">
       <c r="A75" s="8" t="s">
         <v>321</v>
       </c>
@@ -6287,7 +6417,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" ht="16">
       <c r="A76" s="8" t="s">
         <v>321</v>
       </c>
@@ -6344,7 +6474,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" ht="16">
       <c r="A77" s="8" t="s">
         <v>321</v>
       </c>
@@ -6401,7 +6531,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" ht="16">
       <c r="A78" s="8" t="s">
         <v>321</v>
       </c>
@@ -6460,7 +6590,7 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" ht="16">
       <c r="A79" s="8" t="s">
         <v>250</v>
       </c>
@@ -6519,7 +6649,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" ht="16">
       <c r="A80" s="8" t="s">
         <v>250</v>
       </c>
@@ -6578,7 +6708,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" ht="16">
       <c r="A81" s="8" t="s">
         <v>250</v>
       </c>
@@ -6637,7 +6767,7 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" ht="16">
       <c r="A82" s="8" t="s">
         <v>250</v>
       </c>
@@ -6696,7 +6826,7 @@
         <v>2200000</v>
       </c>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" ht="16">
       <c r="A83" s="8" t="s">
         <v>250</v>
       </c>
@@ -6755,7 +6885,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="84" spans="1:19">
+    <row r="84" spans="1:19" ht="16">
       <c r="A84" s="8" t="s">
         <v>250</v>
       </c>
@@ -6812,7 +6942,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="85" spans="1:19">
+    <row r="85" spans="1:19" ht="16">
       <c r="A85" s="8" t="s">
         <v>250</v>
       </c>
@@ -6869,7 +6999,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="86" spans="1:19">
+    <row r="86" spans="1:19" ht="16">
       <c r="A86" s="8" t="s">
         <v>250</v>
       </c>
@@ -6928,7 +7058,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" ht="16">
       <c r="A87" s="8" t="s">
         <v>250</v>
       </c>
@@ -6987,7 +7117,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" ht="16">
       <c r="A88" s="8" t="s">
         <v>250</v>
       </c>
@@ -7046,7 +7176,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:19" ht="16">
       <c r="A89" s="8" t="s">
         <v>250</v>
       </c>
@@ -7105,7 +7235,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" ht="16">
       <c r="A90" s="8" t="s">
         <v>250</v>
       </c>
@@ -7164,7 +7294,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" ht="16">
       <c r="A91" s="8" t="s">
         <v>250</v>
       </c>
@@ -7223,7 +7353,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" ht="16">
       <c r="A92" s="8" t="s">
         <v>250</v>
       </c>
@@ -7282,7 +7412,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" ht="16">
       <c r="A93" s="8" t="s">
         <v>250</v>
       </c>
@@ -7341,7 +7471,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" ht="16">
       <c r="A94" s="8" t="s">
         <v>250</v>
       </c>
@@ -7400,7 +7530,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" ht="16">
       <c r="A95" s="8" t="s">
         <v>250</v>
       </c>
@@ -7459,7 +7589,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" ht="16">
       <c r="A96" s="8" t="s">
         <v>250</v>
       </c>
@@ -7518,7 +7648,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="97" spans="1:19">
+    <row r="97" spans="1:21" ht="16">
       <c r="A97" s="8" t="s">
         <v>250</v>
       </c>
@@ -7577,7 +7707,7 @@
         <v>295000</v>
       </c>
     </row>
-    <row r="98" spans="1:19">
+    <row r="98" spans="1:21" ht="16">
       <c r="A98" s="8" t="s">
         <v>250</v>
       </c>
@@ -7636,17 +7766,417 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="15"/>
-    <row r="100" spans="1:19" ht="15"/>
-    <row r="101" spans="1:19" ht="15"/>
-    <row r="102" spans="1:19" ht="15"/>
-    <row r="103" spans="1:19" ht="15"/>
+    <row r="99" spans="1:21" ht="16">
+      <c r="A99" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B99" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C99" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F99" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G99" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H99" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I99" s="13">
+        <v>9.33</v>
+      </c>
+      <c r="J99" s="13">
+        <v>37.15</v>
+      </c>
+      <c r="K99" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L99" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M99" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N99" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O99" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P99" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q99" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R99" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S99" s="35">
+        <v>15000</v>
+      </c>
+      <c r="T99">
+        <v>15</v>
+      </c>
+      <c r="U99" s="39" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" ht="16">
+      <c r="A100" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C100" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="D100" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G100" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H100" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I100" s="13">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="J100" s="13">
+        <v>48.28</v>
+      </c>
+      <c r="K100" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L100" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M100" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N100" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O100" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P100" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R100" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S100" s="35">
+        <v>45000</v>
+      </c>
+      <c r="T100">
+        <v>45</v>
+      </c>
+      <c r="U100" s="36" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" ht="16">
+      <c r="A101" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C101" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="D101" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G101" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I101" s="13">
+        <v>5.53</v>
+      </c>
+      <c r="J101" s="13">
+        <v>71.3</v>
+      </c>
+      <c r="K101" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L101" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M101" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N101" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P101" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R101" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S101" s="35">
+        <v>65000</v>
+      </c>
+      <c r="T101">
+        <v>65</v>
+      </c>
+      <c r="U101" s="36" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" ht="16">
+      <c r="A102" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B102" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C102" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="D102" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H102" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I102" s="13">
+        <v>25.42</v>
+      </c>
+      <c r="J102" s="13">
+        <v>53.82</v>
+      </c>
+      <c r="K102" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L102" s="13"/>
+      <c r="M102" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N102" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O102" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P102" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q102" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R102" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S102" s="35">
+        <v>180000</v>
+      </c>
+      <c r="T102">
+        <v>180</v>
+      </c>
+      <c r="U102" s="38" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" ht="16">
+      <c r="A103" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C103" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G103" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I103" s="13">
+        <v>1.78</v>
+      </c>
+      <c r="J103" s="13">
+        <v>29.68</v>
+      </c>
+      <c r="K103" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L103" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M103" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N103" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O103" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P103" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q103" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="R103" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S103" s="35">
+        <v>60000</v>
+      </c>
+      <c r="T103"/>
+      <c r="U103" s="36" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" ht="16">
+      <c r="A104" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B104" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C104" s="36" t="s">
+        <v>353</v>
+      </c>
+      <c r="D104" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104" s="13">
+        <v>2019</v>
+      </c>
+      <c r="I104" s="13">
+        <v>2.65</v>
+      </c>
+      <c r="J104" s="13">
+        <v>34.520000000000003</v>
+      </c>
+      <c r="K104" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L104" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M104" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N104" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="O104" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P104" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q104" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="R104" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S104" s="35"/>
+      <c r="T104" s="40"/>
+      <c r="U104" s="36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" ht="16">
+      <c r="A105" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C105" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="D105" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="P105" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S105" s="35">
+        <v>1125000</v>
+      </c>
+      <c r="T105" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="U105" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T98" xr:uid="{CF3E64C5-3E35-4D4B-9072-3C01CE9577D9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T92">
-      <sortCondition ref="D1:D92"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:U98" xr:uid="{3969187F-8484-5348-AE95-011C8946EF44}"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>